<commit_message>
Adding datetime poc for oracle, db2, postgresql.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/datetime-data-types-per-engine.xlsx
+++ b/hotrod/docs/research/datetime-data-types-per-engine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -143,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -164,6 +164,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -266,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -283,6 +290,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,30 +302,34 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -386,19 +401,19 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="35.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,242 +435,242 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" s="7" customFormat="true" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+    <row r="5" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="B6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="B8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="E10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="B12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="B13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="B14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -671,7 +686,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>